<commit_message>
Continue working on import configuration
</commit_message>
<xml_diff>
--- a/tests/data/CompiledDataSet.xlsx
+++ b/tests/data/CompiledDataSet.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite-R\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B0530B-94EF-4509-96AE-0B2D6B36C2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C8BEAE-40EC-443D-ADE9-E6751FF232C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="875" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet_1" sheetId="1" r:id="rId1"/>
-    <sheet name="MetaInfo" sheetId="48" r:id="rId2"/>
-    <sheet name="Stevens_2012_placebo" sheetId="49" r:id="rId3"/>
-    <sheet name="WrongSheet" sheetId="50" r:id="rId4"/>
-    <sheet name="CorrectSheet_additionalCols" sheetId="51" r:id="rId5"/>
-    <sheet name="CorrectSheet_negativeError" sheetId="52" r:id="rId6"/>
+    <sheet name="UnitsFromColumn" sheetId="53" r:id="rId2"/>
+    <sheet name="UnitsFromColumn_secondSheet" sheetId="54" r:id="rId3"/>
+    <sheet name="MetaInfo" sheetId="48" r:id="rId4"/>
+    <sheet name="Stevens_2012_placebo" sheetId="49" r:id="rId5"/>
+    <sheet name="WrongSheet" sheetId="50" r:id="rId6"/>
+    <sheet name="CorrectSheet_additionalCols" sheetId="51" r:id="rId7"/>
+    <sheet name="CorrectSheet_negativeError" sheetId="52" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="78">
   <si>
     <t>Time [h]</t>
   </si>
@@ -431,6 +433,18 @@
   </si>
   <si>
     <t>Sita_dist</t>
+  </si>
+  <si>
+    <t>TimeUnit</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>measurementUnit</t>
+  </si>
+  <si>
+    <t>ng/ml</t>
   </si>
 </sst>
 </file>
@@ -1319,28 +1333,28 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I2" sqref="A1:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1384,7 +1398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1422,7 +1436,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1460,7 +1474,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1498,7 +1512,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1536,7 +1550,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1574,7 +1588,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1612,7 +1626,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1650,7 +1664,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1688,7 +1702,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1726,7 +1740,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1764,7 +1778,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1802,7 +1816,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1846,6 +1860,1281 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFD6957-D35F-4523-AFA1-EEDCE7E2C39C}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="A1:P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="7.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.73046875" customWidth="1"/>
+    <col min="12" max="12" width="23.53125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.53125" customWidth="1"/>
+    <col min="14" max="14" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>480</v>
+      </c>
+      <c r="J2">
+        <v>144.01598816912113</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2">
+        <v>5.5757279200000003</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2">
+        <v>1.238466311</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>480</v>
+      </c>
+      <c r="J3" s="1">
+        <v>144.67036763174102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L3">
+        <v>21.677390540000001</v>
+      </c>
+      <c r="M3" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3">
+        <v>22.807093760000001</v>
+      </c>
+      <c r="O3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>480</v>
+      </c>
+      <c r="J4" s="1">
+        <v>145.3957506816262</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4">
+        <v>37.883090729999999</v>
+      </c>
+      <c r="M4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4">
+        <v>35.70653325</v>
+      </c>
+      <c r="O4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>480</v>
+      </c>
+      <c r="J5">
+        <v>146.03262190864493</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5">
+        <v>27.86415818</v>
+      </c>
+      <c r="O5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>480</v>
+      </c>
+      <c r="J6" s="1">
+        <v>146.60101688784701</v>
+      </c>
+      <c r="K6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6">
+        <v>53.471729979999999</v>
+      </c>
+      <c r="M6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6">
+        <v>24.045102759999999</v>
+      </c>
+      <c r="O6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>480</v>
+      </c>
+      <c r="J7" s="1">
+        <v>147.31270102535808</v>
+      </c>
+      <c r="K7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7">
+        <v>14.964032720000001</v>
+      </c>
+      <c r="O7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>480</v>
+      </c>
+      <c r="J8">
+        <v>148.02467818773277</v>
+      </c>
+      <c r="K8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8">
+        <v>39.235579170000001</v>
+      </c>
+      <c r="M8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8">
+        <v>11.35236649</v>
+      </c>
+      <c r="O8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>480</v>
+      </c>
+      <c r="J9" s="1">
+        <v>148.73634401118989</v>
+      </c>
+      <c r="K9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9">
+        <v>33.66594869</v>
+      </c>
+      <c r="M9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9">
+        <v>10.010472350000001</v>
+      </c>
+      <c r="O9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>480</v>
+      </c>
+      <c r="J10" s="1">
+        <v>149.34127552807428</v>
+      </c>
+      <c r="K10" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10">
+        <v>27.992890379999999</v>
+      </c>
+      <c r="M10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10">
+        <v>8.1528109959999995</v>
+      </c>
+      <c r="O10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>480</v>
+      </c>
+      <c r="J11">
+        <v>150.03481043809506</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11">
+        <v>23.455175430000001</v>
+      </c>
+      <c r="M11" t="s">
+        <v>77</v>
+      </c>
+      <c r="N11">
+        <v>8.5651503859999991</v>
+      </c>
+      <c r="O11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>480</v>
+      </c>
+      <c r="J12" s="1">
+        <v>150.67492325266755</v>
+      </c>
+      <c r="K12" t="s">
+        <v>75</v>
+      </c>
+      <c r="L12">
+        <v>20.258821090000001</v>
+      </c>
+      <c r="M12" t="s">
+        <v>77</v>
+      </c>
+      <c r="N12">
+        <v>8.3592855630000003</v>
+      </c>
+      <c r="O12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>480</v>
+      </c>
+      <c r="J13">
+        <v>168.0165559047943</v>
+      </c>
+      <c r="K13" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13">
+        <v>2.066727336</v>
+      </c>
+      <c r="M13" t="s">
+        <v>77</v>
+      </c>
+      <c r="N13">
+        <v>5.6758783739999998</v>
+      </c>
+      <c r="O13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4F5E7-B3CC-49CB-8009-201040C9557C}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>480</v>
+      </c>
+      <c r="J2">
+        <v>144.01598816912113</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2">
+        <v>5.5757279200000003</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2">
+        <v>1.238466311</v>
+      </c>
+      <c r="O2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>480</v>
+      </c>
+      <c r="J3" s="1">
+        <v>144.67036763174102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L3">
+        <v>21.677390540000001</v>
+      </c>
+      <c r="M3" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3">
+        <v>22.807093760000001</v>
+      </c>
+      <c r="O3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>480</v>
+      </c>
+      <c r="J4" s="1">
+        <v>145.3957506816262</v>
+      </c>
+      <c r="K4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4">
+        <v>37.883090729999999</v>
+      </c>
+      <c r="M4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4">
+        <v>35.70653325</v>
+      </c>
+      <c r="O4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>480</v>
+      </c>
+      <c r="J5">
+        <v>146.03262190864493</v>
+      </c>
+      <c r="K5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5">
+        <v>27.86415818</v>
+      </c>
+      <c r="O5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>480</v>
+      </c>
+      <c r="J6" s="1">
+        <v>146.60101688784701</v>
+      </c>
+      <c r="K6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6">
+        <v>53.471729979999999</v>
+      </c>
+      <c r="M6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6">
+        <v>24.045102759999999</v>
+      </c>
+      <c r="O6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>480</v>
+      </c>
+      <c r="J7" s="1">
+        <v>147.31270102535808</v>
+      </c>
+      <c r="K7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7">
+        <v>14.964032720000001</v>
+      </c>
+      <c r="O7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>480</v>
+      </c>
+      <c r="J8">
+        <v>148.02467818773277</v>
+      </c>
+      <c r="K8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8">
+        <v>39.235579170000001</v>
+      </c>
+      <c r="M8" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8">
+        <v>11.35236649</v>
+      </c>
+      <c r="O8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>480</v>
+      </c>
+      <c r="J9" s="1">
+        <v>148.73634401118989</v>
+      </c>
+      <c r="K9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9">
+        <v>33.66594869</v>
+      </c>
+      <c r="M9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9">
+        <v>10.010472350000001</v>
+      </c>
+      <c r="O9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>480</v>
+      </c>
+      <c r="J10" s="1">
+        <v>149.34127552807428</v>
+      </c>
+      <c r="K10" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10">
+        <v>27.992890379999999</v>
+      </c>
+      <c r="M10" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10">
+        <v>8.1528109959999995</v>
+      </c>
+      <c r="O10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>480</v>
+      </c>
+      <c r="J11">
+        <v>150.03481043809506</v>
+      </c>
+      <c r="K11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11">
+        <v>23.455175430000001</v>
+      </c>
+      <c r="M11" t="s">
+        <v>77</v>
+      </c>
+      <c r="N11">
+        <v>8.5651503859999991</v>
+      </c>
+      <c r="O11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>480</v>
+      </c>
+      <c r="J12" s="1">
+        <v>150.67492325266755</v>
+      </c>
+      <c r="K12" t="s">
+        <v>75</v>
+      </c>
+      <c r="L12">
+        <v>20.258821090000001</v>
+      </c>
+      <c r="M12" t="s">
+        <v>77</v>
+      </c>
+      <c r="N12">
+        <v>8.3592855630000003</v>
+      </c>
+      <c r="O12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>480</v>
+      </c>
+      <c r="J13">
+        <v>168.0165559047943</v>
+      </c>
+      <c r="K13" t="s">
+        <v>75</v>
+      </c>
+      <c r="L13">
+        <v>2.066727336</v>
+      </c>
+      <c r="M13" t="s">
+        <v>77</v>
+      </c>
+      <c r="N13">
+        <v>5.6758783739999998</v>
+      </c>
+      <c r="O13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DF631D-DF5E-4A3F-BA90-F9B6EDEECD77}">
   <dimension ref="C1:I27"/>
   <sheetViews>
@@ -1853,16 +3142,16 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.36328125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.6328125" style="3"/>
+    <col min="1" max="1" width="12.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.59765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1877,7 +3166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1894,7 +3183,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1902,10 +3191,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C8" s="4"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
@@ -1913,10 +3202,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C14" s="4"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -1924,7 +3213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
@@ -1941,7 +3230,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1949,7 +3238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E22" s="3" t="s">
         <v>36</v>
       </c>
@@ -1957,7 +3246,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E23" s="3" t="s">
         <v>37</v>
       </c>
@@ -1965,7 +3254,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1976,7 +3265,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
@@ -1987,7 +3276,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
@@ -2001,7 +3290,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C27" s="3" t="s">
         <v>47</v>
       </c>
@@ -2021,7 +3310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0E8DDA-F3F4-4710-A6B6-93A80B4A8C1A}">
   <dimension ref="A1:N78"/>
   <sheetViews>
@@ -2029,9 +3318,9 @@
       <selection sqref="A1:N78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2075,7 +3364,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -2086,7 +3375,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -2097,7 +3386,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -2108,7 +3397,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -2119,7 +3408,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -2130,7 +3419,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -2141,7 +3430,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -2152,7 +3441,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -2163,7 +3452,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -2174,7 +3463,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -2185,7 +3474,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -2196,7 +3485,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -2207,7 +3496,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -2218,7 +3507,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -2229,7 +3518,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -2240,7 +3529,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -2251,7 +3540,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -2262,7 +3551,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -2273,7 +3562,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -2284,7 +3573,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -2295,7 +3584,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -2306,7 +3595,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -2317,7 +3606,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -2328,7 +3617,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -2339,7 +3628,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -2350,7 +3639,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -2364,7 +3653,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -2378,7 +3667,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -2392,7 +3681,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -2406,7 +3695,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -2420,7 +3709,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -2434,7 +3723,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -2448,7 +3737,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -2462,7 +3751,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -2476,7 +3765,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -2490,7 +3779,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -2504,7 +3793,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -2515,7 +3804,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -2526,7 +3815,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -2540,7 +3829,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -2554,7 +3843,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -2568,7 +3857,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -2582,7 +3871,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -2596,7 +3885,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -2610,7 +3899,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -2624,7 +3913,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -2638,7 +3927,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -2652,7 +3941,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -2666,7 +3955,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -2680,7 +3969,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -2691,7 +3980,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -2702,7 +3991,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -2716,7 +4005,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -2730,7 +4019,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -2744,7 +4033,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -2758,7 +4047,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -2772,7 +4061,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -2786,7 +4075,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -2800,7 +4089,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -2814,7 +4103,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -2828,7 +4117,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -2842,7 +4131,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -2856,7 +4145,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -2870,7 +4159,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -2884,7 +4173,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -2898,7 +4187,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -2912,7 +4201,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -2926,7 +4215,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -2940,7 +4229,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -2954,7 +4243,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -2968,7 +4257,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -2982,7 +4271,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -2996,7 +4285,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -3010,7 +4299,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -3024,7 +4313,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -3038,7 +4327,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -3052,7 +4341,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>
@@ -3071,7 +4360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCB5B98-2408-40BA-99F9-228ECCEE7326}">
   <dimension ref="A1:N1"/>
   <sheetViews>
@@ -3079,9 +4368,9 @@
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3130,7 +4419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C19160-8B30-4C70-A987-7318B15033AF}">
   <dimension ref="A1:Q78"/>
   <sheetViews>
@@ -3138,9 +4427,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3184,7 +4473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -3195,7 +4484,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -3206,7 +4495,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -3217,7 +4506,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -3228,7 +4517,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -3242,7 +4531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -3256,7 +4545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -3270,7 +4559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -3281,7 +4570,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -3292,7 +4581,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -3303,7 +4592,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -3314,7 +4603,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -3325,7 +4614,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -3336,7 +4625,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -3347,7 +4636,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -3358,7 +4647,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -3369,7 +4658,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -3380,7 +4669,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -3391,7 +4680,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -3402,7 +4691,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -3413,7 +4702,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -3424,7 +4713,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -3435,7 +4724,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -3446,7 +4735,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -3457,7 +4746,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -3468,7 +4757,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -3482,7 +4771,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -3496,7 +4785,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -3510,7 +4799,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -3524,7 +4813,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -3538,7 +4827,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -3552,7 +4841,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -3566,7 +4855,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -3580,7 +4869,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -3594,7 +4883,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -3608,7 +4897,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -3622,7 +4911,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -3633,7 +4922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -3644,7 +4933,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -3658,7 +4947,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -3672,7 +4961,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -3686,7 +4975,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -3700,7 +4989,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -3714,7 +5003,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -3728,7 +5017,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -3742,7 +5031,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -3756,7 +5045,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -3770,7 +5059,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -3784,7 +5073,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -3798,7 +5087,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -3809,7 +5098,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -3820,7 +5109,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -3834,7 +5123,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -3848,7 +5137,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -3862,7 +5151,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -3876,7 +5165,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -3890,7 +5179,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -3904,7 +5193,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -3918,7 +5207,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -3932,7 +5221,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -3946,7 +5235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -3960,7 +5249,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -3974,7 +5263,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -3988,7 +5277,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -4002,7 +5291,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -4016,7 +5305,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -4030,7 +5319,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -4044,7 +5333,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -4058,7 +5347,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -4072,7 +5361,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -4086,7 +5375,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -4100,7 +5389,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -4114,7 +5403,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -4128,7 +5417,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -4142,7 +5431,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -4156,7 +5445,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -4170,7 +5459,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>
@@ -4189,17 +5478,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BDD5F-6183-4F95-9E5B-E5759D0B37BB}">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4243,7 +5532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -4254,7 +5543,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -4265,7 +5554,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -4276,7 +5565,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -4287,7 +5576,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -4301,7 +5590,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -4315,7 +5604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -4329,7 +5618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -4340,7 +5629,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -4351,7 +5640,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -4362,7 +5651,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -4373,7 +5662,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -4384,7 +5673,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -4395,7 +5684,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -4406,7 +5695,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -4417,7 +5706,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -4428,7 +5717,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -4439,7 +5728,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -4450,7 +5739,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -4461,7 +5750,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -4472,7 +5761,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -4483,7 +5772,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -4494,7 +5783,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -4505,7 +5794,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -4516,7 +5805,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -4527,7 +5816,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -4541,7 +5830,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -4555,7 +5844,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -4569,7 +5858,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -4583,7 +5872,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -4597,7 +5886,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -4611,7 +5900,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -4625,7 +5914,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -4639,7 +5928,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -4653,7 +5942,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -4667,7 +5956,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -4681,7 +5970,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -4692,7 +5981,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -4703,7 +5992,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -4717,7 +6006,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -4731,7 +6020,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -4745,7 +6034,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -4759,7 +6048,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -4773,7 +6062,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -4787,7 +6076,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -4801,7 +6090,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -4815,7 +6104,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -4829,7 +6118,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -4843,7 +6132,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -4857,7 +6146,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -4868,7 +6157,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -4879,7 +6168,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -4893,7 +6182,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -4907,7 +6196,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -4921,7 +6210,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -4935,7 +6224,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -4949,7 +6238,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -4963,7 +6252,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -4977,7 +6266,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -4991,7 +6280,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -5005,7 +6294,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -5019,7 +6308,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -5033,7 +6322,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -5047,7 +6336,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -5061,7 +6350,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -5075,7 +6364,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -5089,7 +6378,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -5103,7 +6392,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -5117,7 +6406,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -5131,7 +6420,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -5145,7 +6434,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -5159,7 +6448,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -5173,7 +6462,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -5187,7 +6476,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -5201,7 +6490,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -5215,7 +6504,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -5229,7 +6518,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>

</xml_diff>

<commit_message>
Respect encapsulation of UnitDescritpion
</commit_message>
<xml_diff>
--- a/tests/data/CompiledDataSet.xlsx
+++ b/tests/data/CompiledDataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite-R\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C8BEAE-40EC-443D-ADE9-E6751FF232C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DBB84F-0938-4610-BCC3-D0486A73C3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="875" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet_1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="WrongSheet" sheetId="50" r:id="rId6"/>
     <sheet name="CorrectSheet_additionalCols" sheetId="51" r:id="rId7"/>
     <sheet name="CorrectSheet_negativeError" sheetId="52" r:id="rId8"/>
+    <sheet name="DefaultConfig" sheetId="55" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="81">
   <si>
     <t>Time [h]</t>
   </si>
@@ -445,6 +446,15 @@
   </si>
   <si>
     <t>ng/ml</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -1336,25 +1346,25 @@
       <selection activeCell="I2" sqref="A1:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1398,7 +1408,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1436,7 +1446,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1474,7 +1484,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1512,7 +1522,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1550,7 +1560,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1588,7 +1598,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1626,7 +1636,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1664,7 +1674,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1702,7 +1712,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1740,7 +1750,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1778,7 +1788,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1816,7 +1826,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1867,26 +1877,26 @@
       <selection activeCell="M2" sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.9296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.73046875" customWidth="1"/>
-    <col min="12" max="12" width="23.53125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.53125" customWidth="1"/>
-    <col min="14" max="14" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7265625" customWidth="1"/>
+    <col min="12" max="12" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.54296875" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1936,7 +1946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1983,7 +1993,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2030,7 +2040,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2077,7 +2087,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2124,7 +2134,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2171,7 +2181,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2218,7 +2228,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2265,7 +2275,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2312,7 +2322,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2359,7 +2369,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2406,7 +2416,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2453,7 +2463,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2509,13 +2519,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4F5E7-B3CC-49CB-8009-201040C9557C}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2565,7 +2575,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2612,7 +2622,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2659,7 +2669,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2706,7 +2716,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2753,7 +2763,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2800,7 +2810,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2847,7 +2857,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2894,7 +2904,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2941,7 +2951,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2988,7 +2998,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3035,7 +3045,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3082,7 +3092,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -3142,16 +3152,16 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.33203125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.59765625" style="3"/>
+    <col min="1" max="1" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.36328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.36328125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.6328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
@@ -3166,7 +3176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
@@ -3183,7 +3193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
@@ -3191,10 +3201,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C8" s="4"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
@@ -3202,10 +3212,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C14" s="4"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -3213,7 +3223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
@@ -3230,7 +3240,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="E21" s="3" t="s">
         <v>31</v>
       </c>
@@ -3238,7 +3248,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="E22" s="3" t="s">
         <v>36</v>
       </c>
@@ -3246,7 +3256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="E23" s="3" t="s">
         <v>37</v>
       </c>
@@ -3254,7 +3264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
@@ -3265,7 +3275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
@@ -3276,7 +3286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
@@ -3290,7 +3300,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
         <v>47</v>
       </c>
@@ -3318,9 +3328,9 @@
       <selection sqref="A1:N78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3364,7 +3374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J2">
         <v>0</v>
       </c>
@@ -3375,7 +3385,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -3386,7 +3396,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -3397,7 +3407,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -3408,7 +3418,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -3419,7 +3429,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -3430,7 +3440,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -3441,7 +3451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -3452,7 +3462,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -3463,7 +3473,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -3474,7 +3484,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -3485,7 +3495,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -3496,7 +3506,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J14">
         <v>0</v>
       </c>
@@ -3507,7 +3517,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -3518,7 +3528,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -3529,7 +3539,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -3540,7 +3550,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -3551,7 +3561,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -3562,7 +3572,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -3573,7 +3583,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -3584,7 +3594,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -3595,7 +3605,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -3606,7 +3616,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -3617,7 +3627,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -3628,7 +3638,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -3639,7 +3649,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -3653,7 +3663,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -3667,7 +3677,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -3681,7 +3691,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -3695,7 +3705,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -3709,7 +3719,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -3723,7 +3733,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -3737,7 +3747,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -3751,7 +3761,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -3765,7 +3775,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -3779,7 +3789,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -3793,7 +3803,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -3804,7 +3814,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -3815,7 +3825,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -3829,7 +3839,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -3843,7 +3853,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -3857,7 +3867,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -3871,7 +3881,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -3885,7 +3895,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -3899,7 +3909,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -3913,7 +3923,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -3927,7 +3937,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -3941,7 +3951,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -3955,7 +3965,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -3969,7 +3979,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -3980,7 +3990,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -3991,7 +4001,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J53">
         <v>0</v>
       </c>
@@ -4005,7 +4015,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -4019,7 +4029,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -4033,7 +4043,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -4047,7 +4057,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -4061,7 +4071,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -4075,7 +4085,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -4089,7 +4099,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -4103,7 +4113,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J61">
         <v>120</v>
       </c>
@@ -4117,7 +4127,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J62">
         <v>150</v>
       </c>
@@ -4131,7 +4141,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J63">
         <v>180</v>
       </c>
@@ -4145,7 +4155,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -4159,7 +4169,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -4173,7 +4183,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J66">
         <v>0</v>
       </c>
@@ -4187,7 +4197,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -4201,7 +4211,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -4215,7 +4225,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -4229,7 +4239,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -4243,7 +4253,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -4257,7 +4267,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -4271,7 +4281,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -4285,7 +4295,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -4299,7 +4309,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -4313,7 +4323,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J76">
         <v>180</v>
       </c>
@@ -4327,7 +4337,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -4341,7 +4351,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J78">
         <v>240</v>
       </c>
@@ -4368,9 +4378,9 @@
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4427,9 +4437,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4473,7 +4483,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J2">
         <v>0</v>
       </c>
@@ -4484,7 +4494,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -4495,7 +4505,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -4506,7 +4516,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -4517,7 +4527,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -4531,7 +4541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -4545,7 +4555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -4559,7 +4569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -4570,7 +4580,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -4581,7 +4591,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -4592,7 +4602,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -4603,7 +4613,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -4614,7 +4624,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J14">
         <v>0</v>
       </c>
@@ -4625,7 +4635,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -4636,7 +4646,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -4647,7 +4657,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -4658,7 +4668,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -4669,7 +4679,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -4680,7 +4690,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -4691,7 +4701,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -4702,7 +4712,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -4713,7 +4723,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -4724,7 +4734,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -4735,7 +4745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -4746,7 +4756,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -4757,7 +4767,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -4771,7 +4781,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -4785,7 +4795,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -4799,7 +4809,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -4813,7 +4823,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -4827,7 +4837,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -4841,7 +4851,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -4855,7 +4865,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -4869,7 +4879,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -4883,7 +4893,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -4897,7 +4907,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -4911,7 +4921,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -4922,7 +4932,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -4933,7 +4943,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -4947,7 +4957,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -4961,7 +4971,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -4975,7 +4985,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -4989,7 +4999,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -5003,7 +5013,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -5017,7 +5027,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -5031,7 +5041,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -5045,7 +5055,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -5059,7 +5069,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -5073,7 +5083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -5087,7 +5097,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -5098,7 +5108,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -5109,7 +5119,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J53">
         <v>0</v>
       </c>
@@ -5123,7 +5133,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -5137,7 +5147,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -5151,7 +5161,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -5165,7 +5175,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -5179,7 +5189,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -5193,7 +5203,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -5207,7 +5217,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -5221,7 +5231,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J61">
         <v>120</v>
       </c>
@@ -5235,7 +5245,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J62">
         <v>150</v>
       </c>
@@ -5249,7 +5259,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J63">
         <v>180</v>
       </c>
@@ -5263,7 +5273,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -5277,7 +5287,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -5291,7 +5301,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J66">
         <v>0</v>
       </c>
@@ -5305,7 +5315,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -5319,7 +5329,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -5333,7 +5343,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -5347,7 +5357,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -5361,7 +5371,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -5375,7 +5385,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -5389,7 +5399,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -5403,7 +5413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -5417,7 +5427,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -5431,7 +5441,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J76">
         <v>180</v>
       </c>
@@ -5445,7 +5455,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -5459,7 +5469,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J78">
         <v>240</v>
       </c>
@@ -5486,9 +5496,9 @@
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -5532,7 +5542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J2">
         <v>0</v>
       </c>
@@ -5543,7 +5553,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -5554,7 +5564,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -5565,7 +5575,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -5576,7 +5586,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -5590,7 +5600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -5604,7 +5614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -5618,7 +5628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -5629,7 +5639,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -5640,7 +5650,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -5651,7 +5661,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -5662,7 +5672,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -5673,7 +5683,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J14">
         <v>0</v>
       </c>
@@ -5684,7 +5694,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -5695,7 +5705,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -5706,7 +5716,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -5717,7 +5727,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -5728,7 +5738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -5739,7 +5749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -5750,7 +5760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -5761,7 +5771,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -5772,7 +5782,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -5783,7 +5793,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -5794,7 +5804,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -5805,7 +5815,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -5816,7 +5826,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -5830,7 +5840,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -5844,7 +5854,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -5858,7 +5868,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -5872,7 +5882,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -5886,7 +5896,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -5900,7 +5910,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -5914,7 +5924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -5928,7 +5938,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -5942,7 +5952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -5956,7 +5966,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -5970,7 +5980,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -5981,7 +5991,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -5992,7 +6002,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -6006,7 +6016,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -6020,7 +6030,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -6034,7 +6044,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -6048,7 +6058,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -6062,7 +6072,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -6076,7 +6086,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -6090,7 +6100,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -6104,7 +6114,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -6118,7 +6128,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -6132,7 +6142,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -6146,7 +6156,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -6157,7 +6167,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -6168,7 +6178,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J53">
         <v>0</v>
       </c>
@@ -6182,7 +6192,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -6196,7 +6206,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -6210,7 +6220,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -6224,7 +6234,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -6238,7 +6248,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -6252,7 +6262,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -6266,7 +6276,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -6280,7 +6290,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J61">
         <v>120</v>
       </c>
@@ -6294,7 +6304,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J62">
         <v>150</v>
       </c>
@@ -6308,7 +6318,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J63">
         <v>180</v>
       </c>
@@ -6322,7 +6332,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -6336,7 +6346,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -6350,7 +6360,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J66">
         <v>0</v>
       </c>
@@ -6364,7 +6374,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -6378,7 +6388,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -6392,7 +6402,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -6406,7 +6416,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -6420,7 +6430,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -6434,7 +6444,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -6448,7 +6458,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -6462,7 +6472,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -6476,7 +6486,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -6490,7 +6500,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J76">
         <v>180</v>
       </c>
@@ -6504,7 +6514,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -6518,7 +6528,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
       <c r="J78">
         <v>240</v>
       </c>
@@ -6530,6 +6540,43 @@
       </c>
       <c r="N78" t="s">
         <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F0443C-748E-4809-AAEE-9F7977E77C74}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6538,12 +6585,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6764,15 +6808,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6797,17 +6852,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>